<commit_message>
Update of GINF2 Modules
</commit_message>
<xml_diff>
--- a/resources/GINF2/modules.xlsx
+++ b/resources/GINF2/modules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1241C2-B758-41C9-9948-FF81D8482126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A7E163-E32F-431F-A6DE-F70E12D32D2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4C56605D-1814-484D-BD67-6BFC85BD123D}"/>
+    <workbookView xWindow="5760" yWindow="2760" windowWidth="15375" windowHeight="8325" xr2:uid="{4C56605D-1814-484D-BD67-6BFC85BD123D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Code</t>
   </si>
@@ -33,10 +33,139 @@
     <t>Intitulé</t>
   </si>
   <si>
-    <t>Enseignant</t>
-  </si>
-  <si>
-    <t>Nombre d'heures</t>
+    <t>Composants</t>
+  </si>
+  <si>
+    <t>GINF31</t>
+  </si>
+  <si>
+    <t>GINF32</t>
+  </si>
+  <si>
+    <t>GINF33</t>
+  </si>
+  <si>
+    <t>GINF34</t>
+  </si>
+  <si>
+    <t>GINF35</t>
+  </si>
+  <si>
+    <t>GINF36</t>
+  </si>
+  <si>
+    <t>GINF41</t>
+  </si>
+  <si>
+    <t>GINF42</t>
+  </si>
+  <si>
+    <t>GINF43</t>
+  </si>
+  <si>
+    <t>GINF44</t>
+  </si>
+  <si>
+    <t>GINF45</t>
+  </si>
+  <si>
+    <t>GINF46</t>
+  </si>
+  <si>
+    <t>POO &amp; XML</t>
+  </si>
+  <si>
+    <t>Qualité et approche processus</t>
+  </si>
+  <si>
+    <t>Modélisation OO &amp; IHM</t>
+  </si>
+  <si>
+    <t>BD Avancées I</t>
+  </si>
+  <si>
+    <t>Admin. Et prog. Système</t>
+  </si>
+  <si>
+    <t>Langues et Communication</t>
+  </si>
+  <si>
+    <t>Technologies distribués</t>
+  </si>
+  <si>
+    <t>BD Avacncées II &amp; Cloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traitement de l'image </t>
+  </si>
+  <si>
+    <t>Prog. Déclarative et TAV</t>
+  </si>
+  <si>
+    <t>Sécurité des systèmes &amp; Crypto.</t>
+  </si>
+  <si>
+    <t>Management de l'entreprise</t>
+  </si>
+  <si>
+    <t>EL Haddad</t>
+  </si>
+  <si>
+    <t>Badir</t>
+  </si>
+  <si>
+    <t>Ezzine</t>
+  </si>
+  <si>
+    <t>El Alami Hassoun</t>
+  </si>
+  <si>
+    <t>Lazaar</t>
+  </si>
+  <si>
+    <t>El Haddad</t>
+  </si>
+  <si>
+    <t>Ben Achrab</t>
+  </si>
+  <si>
+    <t>Java,XML</t>
+  </si>
+  <si>
+    <t>Qualité, Cycle de vie Logiciel, Optimisation des processus</t>
+  </si>
+  <si>
+    <t>UML,IHM</t>
+  </si>
+  <si>
+    <t>Optimisation BD, Admin. BD, BD Distribuées</t>
+  </si>
+  <si>
+    <t>Ad. Sys, Prog. Sys</t>
+  </si>
+  <si>
+    <t>Anglais, Espagnol</t>
+  </si>
+  <si>
+    <t>J2EE, C#</t>
+  </si>
+  <si>
+    <t>Gestion des données Complexes, NOSQL, Cloud Computing</t>
+  </si>
+  <si>
+    <t>Traitement d'image, vision numérique, Processus stochastique</t>
+  </si>
+  <si>
+    <t>Prog. Déclarative, Technique algorithmique avancée</t>
+  </si>
+  <si>
+    <t>Sécurité des systèmes, Cryptographie</t>
+  </si>
+  <si>
+    <t>Economie &amp; Compta 2, Projets collectifs, Management de projet</t>
+  </si>
+  <si>
+    <t>Chef Module</t>
   </si>
 </sst>
 </file>
@@ -388,13 +517,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9078595-6E23-491B-9A56-4D7BC37B86BD}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -404,10 +538,178 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Issue of Array Same Key Inside Modules
</commit_message>
<xml_diff>
--- a/resources/GINF2/modules.xlsx
+++ b/resources/GINF2/modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2713F034-7CBC-4B45-B7AE-38AC6B2D18EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77814D54-E8C1-4B60-8226-F8A5DE7AD046}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4095" yWindow="1500" windowWidth="15375" windowHeight="8325" xr2:uid="{4C56605D-1814-484D-BD67-6BFC85BD123D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
   <si>
     <t>GINF31</t>
   </si>
@@ -216,7 +216,13 @@
     <t xml:space="preserve"> Management de projet</t>
   </si>
   <si>
-    <t>ElementName</t>
+    <t>ElementName1</t>
+  </si>
+  <si>
+    <t>ElementName2</t>
+  </si>
+  <si>
+    <t>ElementName3</t>
   </si>
 </sst>
 </file>
@@ -570,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9078595-6E23-491B-9A56-4D7BC37B86BD}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,10 +604,10 @@
         <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Field Update : Code
</commit_message>
<xml_diff>
--- a/resources/GINF2/modules.xlsx
+++ b/resources/GINF2/modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Gestion-des-notes-avec-XML\resources\GINF2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77814D54-E8C1-4B60-8226-F8A5DE7AD046}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDBC59C-D640-4C0C-83C7-178156E71AC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4095" yWindow="1500" windowWidth="15375" windowHeight="8325" xr2:uid="{4C56605D-1814-484D-BD67-6BFC85BD123D}"/>
   </bookViews>
@@ -120,9 +120,6 @@
     <t>Ben Achrab</t>
   </si>
   <si>
-    <t>ModuleName</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>ElementName3</t>
+  </si>
+  <si>
+    <t>Code</t>
   </si>
 </sst>
 </file>
@@ -576,9 +576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9078595-6E23-491B-9A56-4D7BC37B86BD}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -592,22 +590,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
       <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>64</v>
-      </c>
-      <c r="F1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -621,10 +619,10 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
         <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -638,13 +636,13 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -658,10 +656,10 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
         <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -675,13 +673,13 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
         <v>41</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -695,10 +693,10 @@
         <v>28</v>
       </c>
       <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
         <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -712,10 +710,10 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
         <v>46</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -729,10 +727,10 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
         <v>48</v>
-      </c>
-      <c r="E8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -746,13 +744,13 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
         <v>50</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>51</v>
-      </c>
-      <c r="F9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -766,13 +764,13 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
         <v>53</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>54</v>
-      </c>
-      <c r="F10" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -786,10 +784,10 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" t="s">
         <v>56</v>
-      </c>
-      <c r="E11" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -803,10 +801,10 @@
         <v>30</v>
       </c>
       <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
         <v>58</v>
-      </c>
-      <c r="E12" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -820,13 +818,13 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" t="s">
         <v>60</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>61</v>
-      </c>
-      <c r="F13" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>